<commit_message>
schema und pin update
</commit_message>
<xml_diff>
--- a/FRDM KL25Z Pin besetzung.xlsx
+++ b/FRDM KL25Z Pin besetzung.xlsx
@@ -391,7 +391,7 @@
     <t>AnschlagHorizontalVorne</t>
   </si>
   <si>
-    <t>DC_DIR_H2</t>
+    <t>DC_SW_H2</t>
   </si>
 </sst>
 </file>
@@ -773,8 +773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>